<commit_message>
Fixed import excel file user_id bug.
</commit_message>
<xml_diff>
--- a/public/uploads/excel_file/file/2/Database.2.xlsx
+++ b/public/uploads/excel_file/file/2/Database.2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26700" windowHeight="15980" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
   <si>
     <t>Form A</t>
   </si>
@@ -237,13 +237,10 @@
     <t>001</t>
   </si>
   <si>
-    <t>LOM-PS</t>
-  </si>
-  <si>
-    <t>PS1-K</t>
-  </si>
-  <si>
-    <t>KAW</t>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>LOM</t>
   </si>
 </sst>
 </file>
@@ -989,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1000,7 +997,7 @@
         <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="3" customFormat="1" ht="28" customHeight="1">
@@ -1082,7 +1079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
@@ -1176,7 +1173,7 @@
         <v>55</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N2" s="5">
         <v>200</v>
@@ -1226,7 +1223,7 @@
         <v>62</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N3" s="5">
         <v>200</v>
@@ -2213,7 +2210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2241,7 +2238,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C2" s="5">
         <v>20</v>
@@ -2255,7 +2252,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C3" s="5">
         <v>25</v>

</xml_diff>